<commit_message>
update images in gitignore
</commit_message>
<xml_diff>
--- a/news_data.xlsx
+++ b/news_data.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,7 +475,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>The two-day or less shipping Americans have come to expect faces a climate change threat</t>
+          <t>Bugs spreading from Europe pose deadly danger to humans, animals and plants, scientists warn</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -485,16 +485,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Many logistics companies have warned about shipping delays due to extreme weather. Weather-related...</t>
+          <t>Disease-carrying bugs from Europe are increasingly crossing the Channel and arriving in Britain as a...</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>images\dc92b58c0add3c2824d94ffae4cc72b5.jpg</t>
+          <t>images\2cbcd37a80811548bc3f263474c83b1f_1.jpg</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -503,22 +503,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>New study suggests climate change will make hail bigger and more costly</t>
+          <t>Naperville teen helps initiate state law requiring climate change be taught in schools</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-08-24</t>
+          <t>2024-08-23</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hail will become less common but larger and more damaging because of human-caused climate change —...</t>
+          <t>Illinois is joining a handful of states across the country that have made climate change education a...</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>images\b0a65647e59cd118a37382aaa01b688e.jpg</t>
+          <t>images\0d7995ef1be281626ac535113afd8f29_1.jpg</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -531,26 +531,26 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Naperville teen helps initiate state law requiring climate change be taught in schools</t>
+          <t>LaMalfa talks Farm Bill, electric vehicles at Wheatland town hall</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-08-23</t>
+          <t>2024-08-24</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Illinois is joining a handful of states across the country that have made climate change education a...</t>
+          <t>Congressman Doug LaMalfa, R-Richvale, made an appearance in Wheatland on Thursday evening as part of a series of town hall meetings throughout the North State, giving local constituents an opportunity ...</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>images\0d7995ef1be281626ac535113afd8f29.jpg</t>
+          <t>No image</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -559,7 +559,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>LaMalfa talks Farm Bill, electric vehicles at Wheatland town hall</t>
+          <t>How candidates for governor would lead on energy, climate change</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -569,16 +569,16 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Congressman Doug LaMalfa, R-Richvale, made an appearance in Wheatland on Thursday evening as part of a series of town hall meetings throughout the North State, giving local constituents an opportunity ...</t>
+          <t>New Hampshire’s natural beauty is undeniable. The next governor of New Hampshire will set the tone...</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>No image</t>
+          <t>images\a56ca3359fcb781e8b777ee15652a732.jpg</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -587,7 +587,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>7 takeaways from the Democratic Party platform on climate</t>
+          <t>New study suggests climate change will make hail bigger and more costly</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -597,7 +597,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>The Democratic Party devoted seven pages of its 90-page 2024 platform to climate policy, offering a...</t>
+          <t>Hail will become less common but larger and more damaging because of human-caused climate change —...</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -615,7 +615,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>How candidates for governor would lead on energy, climate change</t>
+          <t>7 takeaways from the Democratic Party platform on climate</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -625,7 +625,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>New Hampshire’s natural beauty is undeniable. The next governor of New Hampshire will set the tone...</t>
+          <t>The Democratic Party devoted seven pages of its 90-page 2024 platform to climate policy, offering a...</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -643,17 +643,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Was the Sicily yacht hit by a waterspout? Meteorologists explain how climate change fuels storms</t>
+          <t>The two-day or less shipping Americans have come to expect faces a climate change threat</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-08-21</t>
+          <t>2024-08-24</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A superyacht that sank off the coast of Sicily was likely struck by a waterspout made stronger by ...</t>
+          <t>Many logistics companies have warned about shipping delays due to extreme weather. Weather-related...</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -671,17 +671,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Guinness, prosecco, pálinka: Climate change is a serious threat to Europe’s most beloved tipples</t>
+          <t>Was the Sicily yacht hit by a waterspout? Meteorologists explain how climate change fuels storms</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-08-23</t>
+          <t>2024-08-21</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Weather changes aggravated or made more frequent by climate change are endangering some of Europe’s...</t>
+          <t>A superyacht that sank off the coast of Sicily was likely struck by a waterspout made stronger by ...</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -721,6 +721,566 @@
         <v>1</v>
       </c>
       <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Harris’s New Strategy: Equate Fighting Climate Change With ‘Freedom’</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>The Harris campaign isn’t offering details on climate policy but is framing the fight to protect the...</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Guinness, prosecco, pálinka: Climate change is a serious threat to Europe’s most beloved tipples</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Weather changes aggravated or made more frequent by climate change are endangering some of Europe’s...</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>images\6223bbc1f96bc889d01ac5c8462612ef.jpg</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>A climate change storm is coming. Here's how to prepare</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Like an approaching major hurricane whose outer spiral bands are only just beginning to hit, an approaching climate change storm has begun and will soon ...</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Climate change, security take top billing as Pacific Island leaders prepare to meet</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Climate change and security will dominate discussions at next week's meeting of Pacific Islands...</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>images\e7cac736be7f364c0ef7048c712da625.jpg</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Counties with the worst droughts in Tennessee</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2024-08-24</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Have breaking news come to you: Subscribe to News 2 email alerts → Periods of drought have intensified and become more frequent in recent years due to ...</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Climate campaigners are coasting on vibes</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>The energy around Vice President Kamala Harris’ campaign was palpable. “I’m still fired up and giddy with excitement,” said Assembly Utilities and Energy...</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Harris Skips Over Climate Change Even as Party Touts Green Wins</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>(Bloomberg) -- Among the Democrats touting the party’s record confronting climate change at their...</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Series look at regenerative farming, climate change</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2024-08-24</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>The Interfaith Committee of the Cape Ann Climate Coalition is sponsoring five programs this fall addressing climate change. A three-part series focusing ...</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>The Hottest Commodity at the U.S. Open? Shade.</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-08-24</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>The tennis tournament, like the rest of New York City, is adapting to climate change. As New York City contends with rising heat and unpredictable storms...</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Wildfires keep hitting the iconic Pacific Crest Trail, forcing closures and evacuations</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-08-24</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Wildfires are increasingly hitting the Pacific Crest Trail, which runs the length of the West Coast....</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Making the polluter pay is the best way to ‘crack the climate problem’, policy study confirms</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Countless policies have been thrown at the challenge of climate change, but how many have actually...</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>images\0bd7236db1927a85eff23d8f6b014432.jpg</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Glastonbury gets 'climate action plan'</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Glastonbury's community has put together a town climate plan [PA Media] Glastonbury residents have created a bespoke plan to help the town deal with the...</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>images\aba0840fa7621e39d514807a21123e5e.jpg</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Weekend Warm-Up: Another View of the Matterhorn's Dangerous Descent » Explorersweb</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2024-08-24</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>It has been a tough summer season in the Alps. Rockfall is increasing as climate change melts the...</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>images\3b03526b320fde5bdd5e48bcc445a065.jpg</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>UN Report Calls For Businesses To Pay For Climate Change, Restructuring Of Economy</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>A new United Nation’s report examines the costs and impacts of climate change, making drastic...</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Climate change stalling cleanup of Boston rivers, EPA report card says</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Improvements to Boston’s three major rivers are slowing or stalled, and climate change is a major...</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>What has worked to fight climate change? Policies where someone pays for polluting, study finds</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>To figure out what really works when nations try to fight climate change, researchers looked at...</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Why Democrats are so quiet about climate change right now</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2024-08-22</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Vice President Kamala Harris and other Democrats have not made significant mentions of climate ...</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>What has worked to fight climate change? Policies where someone pays for polluting, study finds</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2024-08-22</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>WASHINGTON (AP) — To figure out what really works when nations try to fight climate change,...</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Forum: How, late in life, I understood gravity of climate change | HeraldNet.com</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2024-08-24</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Editor’s note: Jim Bloss, a Monroe resident, and regular contributor to The Herald’s letters to the editor column and Herald Forum, died on Aug. 15. Then I heard the plea of the young Swedish ...</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>No image</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Harris, Walz briefly frame climate change in context of "freedom"</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>There's a striking consistency in the way Kamala Harris and Tim Walz offered just glancing...</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>images\b0cfad057ab09672b28ff6a126df8457.jpg</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>